<commit_message>
multiple root support and expand after save entitiy
</commit_message>
<xml_diff>
--- a/resources/Time_Sheet.xlsx
+++ b/resources/Time_Sheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="900" yWindow="460" windowWidth="24700" windowHeight="15540"/>
+    <workbookView xWindow="920" yWindow="460" windowWidth="24680" windowHeight="15540"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="17" r:id="rId1"/>
@@ -627,7 +627,7 @@
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
+      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" outlineLevelRow="1" x14ac:dyDescent="0.15"/>

</xml_diff>